<commit_message>
recompute all beach slopes
</commit_message>
<xml_diff>
--- a/data/nzd0001/nzd0001.xlsx
+++ b/data/nzd0001/nzd0001.xlsx
@@ -23266,13 +23266,13 @@
         <v>1</v>
       </c>
       <c r="F2" t="n">
-        <v>0.05</v>
+        <v>0.1</v>
       </c>
       <c r="G2" t="n">
-        <v>0.0397</v>
+        <v>0.0636</v>
       </c>
       <c r="H2" t="n">
-        <v>0.0679</v>
+        <v>0.2</v>
       </c>
       <c r="I2" t="n">
         <v>-0.04800674239868728</v>
@@ -23343,9 +23343,15 @@
       <c r="E3" t="n">
         <v>0.9687278939015731</v>
       </c>
-      <c r="F3" t="inlineStr"/>
-      <c r="G3" t="inlineStr"/>
-      <c r="H3" t="inlineStr"/>
+      <c r="F3" t="n">
+        <v>0.105</v>
+      </c>
+      <c r="G3" t="n">
+        <v>0.06950000000000001</v>
+      </c>
+      <c r="H3" t="n">
+        <v>0.2</v>
+      </c>
       <c r="I3" t="n">
         <v>-0.1931154215473095</v>
       </c>
@@ -23416,13 +23422,13 @@
         <v>0.9374557878043063</v>
       </c>
       <c r="F4" t="n">
-        <v>0.06</v>
+        <v>0.12</v>
       </c>
       <c r="G4" t="n">
-        <v>0.0478</v>
+        <v>0.0757</v>
       </c>
       <c r="H4" t="n">
-        <v>0.0776</v>
+        <v>0.2</v>
       </c>
       <c r="I4" t="n">
         <v>-0.2805125119116255</v>
@@ -23493,9 +23499,15 @@
       <c r="E5" t="n">
         <v>0.9061836817070442</v>
       </c>
-      <c r="F5" t="inlineStr"/>
-      <c r="G5" t="inlineStr"/>
-      <c r="H5" t="inlineStr"/>
+      <c r="F5" t="n">
+        <v>0.065</v>
+      </c>
+      <c r="G5" t="n">
+        <v>0.0546</v>
+      </c>
+      <c r="H5" t="n">
+        <v>0.0759</v>
+      </c>
       <c r="I5" t="n">
         <v>-0.319369704220235</v>
       </c>
@@ -23566,13 +23578,13 @@
         <v>0.8749115756086124</v>
       </c>
       <c r="F6" t="n">
-        <v>0.055</v>
+        <v>0.065</v>
       </c>
       <c r="G6" t="n">
-        <v>0.045</v>
+        <v>0.0567</v>
       </c>
       <c r="H6" t="n">
-        <v>0.0664</v>
+        <v>0.0788</v>
       </c>
       <c r="I6" t="n">
         <v>-0.3858886746465036</v>
@@ -23643,9 +23655,15 @@
       <c r="E7" t="n">
         <v>0.8436394695113504</v>
       </c>
-      <c r="F7" t="inlineStr"/>
-      <c r="G7" t="inlineStr"/>
-      <c r="H7" t="inlineStr"/>
+      <c r="F7" t="n">
+        <v>0.07000000000000001</v>
+      </c>
+      <c r="G7" t="n">
+        <v>0.0605</v>
+      </c>
+      <c r="H7" t="n">
+        <v>0.0851</v>
+      </c>
       <c r="I7" t="n">
         <v>-0.3849345781447092</v>
       </c>
@@ -23716,13 +23734,13 @@
         <v>0.8123673634129187</v>
       </c>
       <c r="F8" t="n">
+        <v>0.075</v>
+      </c>
+      <c r="G8" t="n">
         <v>0.065</v>
       </c>
-      <c r="G8" t="n">
-        <v>0.0571</v>
-      </c>
       <c r="H8" t="n">
-        <v>0.08119999999999999</v>
+        <v>0.0916</v>
       </c>
       <c r="I8" t="n">
         <v>-0.3555615266396187</v>
@@ -23794,13 +23812,13 @@
         <v>0.7816450504320696</v>
       </c>
       <c r="F9" t="n">
-        <v>0.06</v>
+        <v>0.075</v>
       </c>
       <c r="G9" t="n">
-        <v>0.0525</v>
+        <v>0.063</v>
       </c>
       <c r="H9" t="n">
-        <v>0.0722</v>
+        <v>0.0885</v>
       </c>
       <c r="I9" t="n">
         <v>-0.2729819206469458</v>
@@ -23872,13 +23890,13 @@
         <v>0.7503729443345427</v>
       </c>
       <c r="F10" t="n">
-        <v>0.065</v>
+        <v>0.08</v>
       </c>
       <c r="G10" t="n">
-        <v>0.054</v>
+        <v>0.07149999999999999</v>
       </c>
       <c r="H10" t="n">
-        <v>0.07530000000000001</v>
+        <v>0.09760000000000001</v>
       </c>
       <c r="I10" t="n">
         <v>-0.2540737872909737</v>
@@ -23950,13 +23968,13 @@
         <v>0.7191008382369553</v>
       </c>
       <c r="F11" t="n">
-        <v>0.065</v>
+        <v>0.08</v>
       </c>
       <c r="G11" t="n">
-        <v>0.0561</v>
+        <v>0.0687</v>
       </c>
       <c r="H11" t="n">
-        <v>0.076</v>
+        <v>0.09039999999999999</v>
       </c>
       <c r="I11" t="n">
         <v>-0.2687612205850651</v>
@@ -24028,13 +24046,13 @@
         <v>0.6878287321393679</v>
       </c>
       <c r="F12" t="n">
-        <v>0.065</v>
+        <v>0.08</v>
       </c>
       <c r="G12" t="n">
-        <v>0.0572</v>
+        <v>0.068</v>
       </c>
       <c r="H12" t="n">
-        <v>0.0805</v>
+        <v>0.0915</v>
       </c>
       <c r="I12" t="n">
         <v>-0.2571659270862445</v>
@@ -24106,13 +24124,13 @@
         <v>0.6565566260419015</v>
       </c>
       <c r="F13" t="n">
-        <v>0.075</v>
+        <v>0.07000000000000001</v>
       </c>
       <c r="G13" t="n">
-        <v>0.06469999999999999</v>
+        <v>0.056</v>
       </c>
       <c r="H13" t="n">
-        <v>0.0945</v>
+        <v>0.0859</v>
       </c>
       <c r="I13" t="n">
         <v>-0.2330910679456993</v>
@@ -24184,13 +24202,13 @@
         <v>0.6252845199441931</v>
       </c>
       <c r="F14" t="n">
-        <v>0.08</v>
+        <v>0.075</v>
       </c>
       <c r="G14" t="n">
-        <v>0.0694</v>
+        <v>0.068</v>
       </c>
       <c r="H14" t="n">
-        <v>0.0956</v>
+        <v>0.08500000000000001</v>
       </c>
       <c r="I14" t="n">
         <v>-0.1382018101204556</v>
@@ -24262,13 +24280,13 @@
         <v>0.5940124138467268</v>
       </c>
       <c r="F15" t="n">
-        <v>0.075</v>
+        <v>0.08</v>
       </c>
       <c r="G15" t="n">
-        <v>0.0645</v>
+        <v>0.06519999999999999</v>
       </c>
       <c r="H15" t="n">
-        <v>0.0864</v>
+        <v>0.0979</v>
       </c>
       <c r="I15" t="n">
         <v>-0.125964421061364</v>
@@ -24340,13 +24358,13 @@
         <v>0.5627536669221561</v>
       </c>
       <c r="F16" t="n">
-        <v>0.075</v>
+        <v>0.08</v>
       </c>
       <c r="G16" t="n">
-        <v>0.06469999999999999</v>
+        <v>0.0644</v>
       </c>
       <c r="H16" t="n">
-        <v>0.0858</v>
+        <v>0.1065</v>
       </c>
       <c r="I16" t="n">
         <v>-0.1091667459769166</v>
@@ -24418,13 +24436,13 @@
         <v>0.5314815608238754</v>
       </c>
       <c r="F17" t="n">
-        <v>0.08</v>
+        <v>0.075</v>
       </c>
       <c r="G17" t="n">
-        <v>0.0698</v>
+        <v>0.0694</v>
       </c>
       <c r="H17" t="n">
-        <v>0.0916</v>
+        <v>0.0872</v>
       </c>
       <c r="I17" t="n">
         <v>-0.1098658734969039</v>
@@ -24499,10 +24517,10 @@
         <v>0.08500000000000001</v>
       </c>
       <c r="G18" t="n">
-        <v>0.07190000000000001</v>
+        <v>0.0747</v>
       </c>
       <c r="H18" t="n">
-        <v>0.0975</v>
+        <v>0.093</v>
       </c>
       <c r="I18" t="n">
         <v>-0.03439301670562504</v>
@@ -24577,10 +24595,10 @@
         <v>0.09</v>
       </c>
       <c r="G19" t="n">
-        <v>0.0775</v>
+        <v>0.0784</v>
       </c>
       <c r="H19" t="n">
-        <v>0.1023</v>
+        <v>0.1</v>
       </c>
       <c r="I19" t="n">
         <v>0.05781367581033135</v>
@@ -24652,13 +24670,13 @@
         <v>0.4376652425311265</v>
       </c>
       <c r="F20" t="n">
-        <v>0.09</v>
+        <v>0.08500000000000001</v>
       </c>
       <c r="G20" t="n">
-        <v>0.0752</v>
+        <v>0.07290000000000001</v>
       </c>
       <c r="H20" t="n">
-        <v>0.1055</v>
+        <v>0.09619999999999999</v>
       </c>
       <c r="I20" t="n">
         <v>0.02374047639677126</v>
@@ -24730,13 +24748,13 @@
         <v>0.4063931364329183</v>
       </c>
       <c r="F21" t="n">
-        <v>0.08500000000000001</v>
+        <v>0.08</v>
       </c>
       <c r="G21" t="n">
-        <v>0.0733</v>
+        <v>0.0649</v>
       </c>
       <c r="H21" t="n">
-        <v>0.1071</v>
+        <v>0.0994</v>
       </c>
       <c r="I21" t="n">
         <v>0.01781775453439549</v>
@@ -24808,13 +24826,13 @@
         <v>0.3751210303355755</v>
       </c>
       <c r="F22" t="n">
-        <v>0.1</v>
+        <v>0.09</v>
       </c>
       <c r="G22" t="n">
-        <v>0.0828</v>
+        <v>0.07539999999999999</v>
       </c>
       <c r="H22" t="n">
-        <v>0.1321</v>
+        <v>0.1052</v>
       </c>
       <c r="I22" t="n">
         <v>-0.06948572265096395</v>
@@ -24886,13 +24904,13 @@
         <v>0.3438489242383777</v>
       </c>
       <c r="F23" t="n">
-        <v>0.09</v>
+        <v>0.08500000000000001</v>
       </c>
       <c r="G23" t="n">
-        <v>0.0731</v>
+        <v>0.073</v>
       </c>
       <c r="H23" t="n">
-        <v>0.1099</v>
+        <v>0.09909999999999999</v>
       </c>
       <c r="I23" t="n">
         <v>-0.05726440516009759</v>
@@ -24964,13 +24982,13 @@
         <v>0.3127028338592166</v>
       </c>
       <c r="F24" t="n">
-        <v>0.08500000000000001</v>
+        <v>0.095</v>
       </c>
       <c r="G24" t="n">
-        <v>0.0699</v>
+        <v>0.0839</v>
       </c>
       <c r="H24" t="n">
-        <v>0.1039</v>
+        <v>0.1149</v>
       </c>
       <c r="I24" t="n">
         <v>-0.03875453405679951</v>
@@ -25042,13 +25060,13 @@
         <v>0.2814307277619801</v>
       </c>
       <c r="F25" t="n">
-        <v>0.08500000000000001</v>
+        <v>0.095</v>
       </c>
       <c r="G25" t="n">
-        <v>0.0722</v>
+        <v>0.0784</v>
       </c>
       <c r="H25" t="n">
-        <v>0.0977</v>
+        <v>0.118</v>
       </c>
       <c r="I25" t="n">
         <v>0.01836350131854391</v>
@@ -25120,13 +25138,13 @@
         <v>0.2501586216640487</v>
       </c>
       <c r="F26" t="n">
-        <v>0.08500000000000001</v>
+        <v>0.095</v>
       </c>
       <c r="G26" t="n">
-        <v>0.07240000000000001</v>
+        <v>0.0815</v>
       </c>
       <c r="H26" t="n">
-        <v>0.1084</v>
+        <v>0.1168</v>
       </c>
       <c r="I26" t="n">
         <v>0.05099870044464118</v>
@@ -25198,13 +25216,13 @@
         <v>0.2188865155659276</v>
       </c>
       <c r="F27" t="n">
-        <v>0.1</v>
+        <v>0.08500000000000001</v>
       </c>
       <c r="G27" t="n">
-        <v>0.0785</v>
+        <v>0.06619999999999999</v>
       </c>
       <c r="H27" t="n">
-        <v>0.1331</v>
+        <v>0.1255</v>
       </c>
       <c r="I27" t="n">
         <v>0.1800517489300072</v>
@@ -25279,10 +25297,10 @@
         <v>0.1</v>
       </c>
       <c r="G28" t="n">
-        <v>0.07679999999999999</v>
+        <v>0.0818</v>
       </c>
       <c r="H28" t="n">
-        <v>0.1354</v>
+        <v>0.1322</v>
       </c>
       <c r="I28" t="n">
         <v>0.343043766743351</v>
@@ -25354,13 +25372,13 @@
         <v>0.1563423033703806</v>
       </c>
       <c r="F29" t="n">
-        <v>0.1</v>
+        <v>0.115</v>
       </c>
       <c r="G29" t="n">
-        <v>0.073</v>
+        <v>0.0912</v>
       </c>
       <c r="H29" t="n">
-        <v>0.1497</v>
+        <v>0.1531</v>
       </c>
       <c r="I29" t="n">
         <v>0.3282708884151369</v>
@@ -25432,13 +25450,13 @@
         <v>0.1250701972734284</v>
       </c>
       <c r="F30" t="n">
-        <v>0.1</v>
+        <v>0.15</v>
       </c>
       <c r="G30" t="n">
-        <v>0.0771</v>
+        <v>0.1068</v>
       </c>
       <c r="H30" t="n">
-        <v>0.1533</v>
+        <v>0.2</v>
       </c>
       <c r="I30" t="n">
         <v>0.4934926714711931</v>
@@ -25510,13 +25528,13 @@
         <v>0.09381631829357515</v>
       </c>
       <c r="F31" t="n">
-        <v>0.14</v>
+        <v>0.125</v>
       </c>
       <c r="G31" t="n">
-        <v>0.0915</v>
+        <v>0.09429999999999999</v>
       </c>
       <c r="H31" t="n">
-        <v>0.2</v>
+        <v>0.1867</v>
       </c>
       <c r="I31" t="n">
         <v>0.3726128033776709</v>
@@ -25588,13 +25606,13 @@
         <v>0.06254421219578769</v>
       </c>
       <c r="F32" t="n">
-        <v>0.135</v>
+        <v>0.12</v>
       </c>
       <c r="G32" t="n">
-        <v>0.0885</v>
+        <v>0.0901</v>
       </c>
       <c r="H32" t="n">
-        <v>0.2</v>
+        <v>0.1705</v>
       </c>
       <c r="I32" t="n">
         <v>0.2939980916304272</v>
@@ -25666,13 +25684,13 @@
         <v>0.03127210609789385</v>
       </c>
       <c r="F33" t="n">
-        <v>0.1</v>
+        <v>0.11</v>
       </c>
       <c r="G33" t="n">
-        <v>0.0725</v>
+        <v>0.08459999999999999</v>
       </c>
       <c r="H33" t="n">
-        <v>0.1503</v>
+        <v>0.154</v>
       </c>
       <c r="I33" t="n">
         <v>0.3357740664586535</v>
@@ -25744,13 +25762,13 @@
         <v>0</v>
       </c>
       <c r="F34" t="n">
-        <v>0.1</v>
+        <v>0.11</v>
       </c>
       <c r="G34" t="n">
-        <v>0.0742</v>
+        <v>0.08400000000000001</v>
       </c>
       <c r="H34" t="n">
-        <v>0.157</v>
+        <v>0.1518</v>
       </c>
       <c r="I34" t="n">
         <v>0.2222485884041857</v>

</xml_diff>